<commit_message>
Generacion de atributo recta curva
</commit_message>
<xml_diff>
--- a/coordenadas autodromo.xlsx
+++ b/coordenadas autodromo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elchi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elchi\Desktop\programacion\Python\F1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D001CC-43A0-42A2-B7A0-5B758D72E87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1904CEC1-8303-4974-87EC-32D85A3F7A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4845" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{B849C1EF-5BD0-4E9A-BBE2-BF88FD870208}"/>
+    <workbookView xWindow="14295" yWindow="7965" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{B849C1EF-5BD0-4E9A-BBE2-BF88FD870208}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3077" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3141" uniqueCount="13">
   <si>
     <t>X</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>recta</t>
+  </si>
+  <si>
+    <t>curva</t>
   </si>
 </sst>
 </file>
@@ -9975,10 +9981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9AB454-6F43-457B-9974-E2CF1EB09CAF}">
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12211,7 +12217,7 @@
         <v>-996.43330000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -12231,7 +12237,7 @@
         <v>-994.65359999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>0</v>
       </c>
@@ -12251,7 +12257,7 @@
         <v>-992.87400000000002</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -12271,7 +12277,7 @@
         <v>-971.44129999999996</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -12291,7 +12297,7 @@
         <v>-950.00850000000003</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -12311,7 +12317,7 @@
         <v>-928.57579999999996</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -12331,7 +12337,7 @@
         <v>-925.28189999999995</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -12351,7 +12357,7 @@
         <v>-921.98800000000006</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -12371,7 +12377,7 @@
         <v>-918.69410000000005</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -12391,7 +12397,7 @@
         <v>-916.11919999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -12411,7 +12417,7 @@
         <v>-913.54430000000002</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -12431,7 +12437,7 @@
         <v>-910.96939999999995</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -12451,7 +12457,7 @@
         <v>-901.94349999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -12471,7 +12477,7 @@
         <v>-892.91759999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -12491,7 +12497,7 @@
         <v>-883.89170000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -12510,8 +12516,11 @@
       <c r="F127">
         <v>-880.8175</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -12530,8 +12539,11 @@
       <c r="F128">
         <v>-877.74329999999998</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -12550,8 +12562,11 @@
       <c r="F129">
         <v>-874.66909999999996</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -12570,8 +12585,11 @@
       <c r="F130">
         <v>-871.77359999999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -12590,8 +12608,11 @@
       <c r="F131">
         <v>-868.87810000000002</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -12610,8 +12631,11 @@
       <c r="F132">
         <v>-865.98260000000005</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -12630,8 +12654,11 @@
       <c r="F133">
         <v>-831.3546</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>0</v>
       </c>
@@ -12650,8 +12677,11 @@
       <c r="F134">
         <v>-796.72659999999996</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -12670,8 +12700,11 @@
       <c r="F135">
         <v>-762.09860000000003</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -12690,8 +12723,11 @@
       <c r="F136">
         <v>-697.12559999999996</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -12710,8 +12746,11 @@
       <c r="F137">
         <v>-632.15250000000003</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -12730,8 +12769,11 @@
       <c r="F138">
         <v>-567.17939999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -12750,8 +12792,11 @@
       <c r="F139">
         <v>-520.80949999999996</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -12770,8 +12815,11 @@
       <c r="F140">
         <v>-474.43959999999998</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -12790,8 +12838,11 @@
       <c r="F141">
         <v>-428.06959999999998</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -12810,8 +12861,11 @@
       <c r="F142">
         <v>-423.14100000000002</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -12830,8 +12884,11 @@
       <c r="F143">
         <v>-418.21249999999998</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -12850,8 +12907,11 @@
       <c r="F144">
         <v>-413.28390000000002</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -12870,8 +12930,11 @@
       <c r="F145">
         <v>-408.28129999999999</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -12890,8 +12953,11 @@
       <c r="F146">
         <v>-403.27870000000001</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -12910,8 +12976,11 @@
       <c r="F147">
         <v>-398.27609999999999</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -12930,8 +12999,11 @@
       <c r="F148">
         <v>-388.27800000000002</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -12950,8 +13022,11 @@
       <c r="F149">
         <v>-378.27980000000002</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -12970,8 +13045,11 @@
       <c r="F150">
         <v>-368.28160000000003</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G150" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -12990,8 +13068,11 @@
       <c r="F151">
         <v>-359.78809999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G151" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -13010,8 +13091,11 @@
       <c r="F152">
         <v>-351.29450000000003</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G152" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -13030,8 +13114,11 @@
       <c r="F153">
         <v>-342.80090000000001</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -13050,8 +13137,11 @@
       <c r="F154">
         <v>-330.8374</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G154" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -13070,8 +13160,11 @@
       <c r="F155">
         <v>-318.87389999999999</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G155" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -13090,8 +13183,11 @@
       <c r="F156">
         <v>-306.91039999999998</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G156" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -13110,8 +13206,11 @@
       <c r="F157">
         <v>-301.68799999999999</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G157" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -13130,8 +13229,11 @@
       <c r="F158">
         <v>-296.46550000000002</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G158" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -13150,8 +13252,11 @@
       <c r="F159">
         <v>-291.24310000000003</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G159" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -13170,8 +13275,11 @@
       <c r="F160">
         <v>-286.91860000000003</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -13190,8 +13298,11 @@
       <c r="F161">
         <v>-282.59410000000003</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G161" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -13210,8 +13321,11 @@
       <c r="F162">
         <v>-278.26960000000003</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G162" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -13230,8 +13344,11 @@
       <c r="F163">
         <v>-274.24770000000001</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G163" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -13250,8 +13367,11 @@
       <c r="F164">
         <v>-270.22579999999999</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G164" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -13270,8 +13390,11 @@
       <c r="F165">
         <v>-266.20389999999998</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G165" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -13290,8 +13413,11 @@
       <c r="F166">
         <v>-262.28609999999998</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G166" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -13310,8 +13436,11 @@
       <c r="F167">
         <v>-258.36829999999998</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G167" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -13330,8 +13459,11 @@
       <c r="F168">
         <v>-254.45050000000001</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G168" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -13350,8 +13482,11 @@
       <c r="F169">
         <v>-246.45079999999999</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G169" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -13370,8 +13505,11 @@
       <c r="F170">
         <v>-238.4511</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G170" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -13390,8 +13528,11 @@
       <c r="F171">
         <v>-230.45150000000001</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G171" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>0</v>
       </c>
@@ -13410,8 +13551,11 @@
       <c r="F172">
         <v>-216.2011</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G172" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -13430,8 +13574,11 @@
       <c r="F173">
         <v>-201.95079999999999</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G173" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -13450,136 +13597,187 @@
       <c r="F174">
         <v>-187.7004</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G174" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C175">
         <v>1306.3993</v>
       </c>
       <c r="F175">
         <v>-187.7004</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G175" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C176">
         <v>1305.2058999999999</v>
       </c>
       <c r="F176">
         <v>-182.1507</v>
       </c>
-    </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G176" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C177">
         <v>1304.0125</v>
       </c>
       <c r="F177">
         <v>-176.601</v>
       </c>
-    </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G177" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C178">
         <v>1302.819</v>
       </c>
       <c r="F178">
         <v>-171.0513</v>
       </c>
-    </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G178" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C179">
         <v>1283.1514</v>
       </c>
       <c r="F179">
         <v>-166.95849999999999</v>
       </c>
-    </row>
-    <row r="180" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G179" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C180">
         <v>1263.4837</v>
       </c>
       <c r="F180">
         <v>-162.8657</v>
       </c>
-    </row>
-    <row r="181" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G180" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C181">
         <v>1243.816</v>
       </c>
       <c r="F181">
         <v>-158.77279999999999</v>
       </c>
-    </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G181" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="182" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C182">
         <v>1079.9593</v>
       </c>
       <c r="F182">
         <v>-136.12</v>
       </c>
-    </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C183">
         <v>916.10260000000005</v>
       </c>
       <c r="F183">
         <v>-113.46720000000001</v>
       </c>
-    </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G183" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C184">
         <v>752.24590000000001</v>
       </c>
       <c r="F184">
         <v>-90.814400000000006</v>
       </c>
-    </row>
-    <row r="185" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G184" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C185">
         <v>645.47469999999998</v>
       </c>
       <c r="F185">
         <v>-79.470500000000001</v>
       </c>
-    </row>
-    <row r="186" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G185" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C186">
         <v>538.70339999999999</v>
       </c>
       <c r="F186">
         <v>-68.126499999999993</v>
       </c>
-    </row>
-    <row r="187" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G186" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C187">
         <v>431.93220000000002</v>
       </c>
       <c r="F187">
         <v>-56.782600000000002</v>
       </c>
-    </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G187" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="188" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C188">
         <v>287.95479999999998</v>
       </c>
       <c r="F188">
         <v>-37.854999999999997</v>
       </c>
-    </row>
-    <row r="189" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G188" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="189" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C189">
         <v>143.97739999999999</v>
       </c>
       <c r="F189">
         <v>-18.927499999999998</v>
       </c>
-    </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G189" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C190">
         <v>0</v>
       </c>
       <c r="F190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G190" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C191">
         <v>-7.5636999999999999</v>
       </c>
@@ -13587,7 +13785,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="192" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C192">
         <v>-15.1274</v>
       </c>

</xml_diff>